<commit_message>
Fix #12728 - [Bug] Maj citeo report theme
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportCiteo.xlsx
@@ -12,10 +12,15 @@
     <sheet name="Matériaux" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -414,7 +419,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -476,6 +481,15 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -484,6 +498,13 @@
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FFCCCCCC"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -503,7 +524,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,20 +533,86 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF004254"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF7F7F7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009FE3"/>
+        <bgColor rgb="FF00B2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2987A"/>
+        <bgColor rgb="FFED7483"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DC799"/>
+        <bgColor rgb="FFA7D2AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7483"/>
+        <bgColor rgb="FFF2987A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B2CC"/>
+        <bgColor rgb="FF009FE3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80CEF4"/>
+        <bgColor rgb="FF66CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD17A"/>
+        <bgColor rgb="FFF7C7CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7D2AE"/>
+        <bgColor rgb="FF8DC799"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7C7CD"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor rgb="FF80CEF4"/>
       </patternFill>
     </fill>
   </fills>
@@ -707,7 +794,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -724,7 +811,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,99 +819,115 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,11 +935,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -864,17 +967,17 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF009FE3"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF8DC799"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFED7483"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -883,23 +986,23 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF00B2CC"/>
+      <rgbColor rgb="FFA7D2AE"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF80CEF4"/>
+      <rgbColor rgb="FFF2987A"/>
+      <rgbColor rgb="FFF7C7CD"/>
+      <rgbColor rgb="FFFDD17A"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF66CCFF"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF004254"/>
+      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -923,7 +1026,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -934,8 +1037,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33599520" y="290520"/>
-          <a:ext cx="178200" cy="360"/>
+          <a:off x="33595560" y="290520"/>
+          <a:ext cx="178560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -996,7 +1099,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1013,7 +1116,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1024,8 +1127,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33599520" y="290520"/>
-          <a:ext cx="178200" cy="360"/>
+          <a:off x="33595560" y="290520"/>
+          <a:ext cx="178560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1086,7 +1189,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1103,7 +1206,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1114,8 +1217,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33599520" y="290520"/>
-          <a:ext cx="178200" cy="360"/>
+          <a:off x="33595560" y="290520"/>
+          <a:ext cx="178560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1176,7 +1279,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1193,7 +1296,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1204,8 +1307,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33599520" y="290520"/>
-          <a:ext cx="178200" cy="360"/>
+          <a:off x="33595560" y="290520"/>
+          <a:ext cx="178560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1266,7 +1369,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1292,7 +1395,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
@@ -1479,7 +1582,7 @@
       <c r="AMG3" s="13"/>
       <c r="AMH3" s="13"/>
       <c r="AMI3" s="13"/>
-      <c r="AMJ3" s="14"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -1494,25 +1597,25 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18" t="s">
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="16"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
@@ -1526,9 +1629,9 @@
       <c r="AL4" s="12"/>
       <c r="AM4" s="12"/>
       <c r="AN4" s="12"/>
-      <c r="AMJ4" s="14"/>
+      <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="14" customFormat="true" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1541,35 +1644,35 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="7"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="19"/>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="7" t="s">
+      <c r="N5" s="20"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7" t="s">
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="10" t="s">
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10" t="s">
+      <c r="W5" s="20"/>
+      <c r="X5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
@@ -1584,125 +1687,125 @@
       <c r="AM5" s="12"/>
       <c r="AN5" s="12"/>
     </row>
-    <row r="6" s="21" customFormat="true" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+    <row r="6" s="22" customFormat="true" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="24" t="s">
+      <c r="M6" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="Q6" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="R6" s="24" t="s">
+      <c r="R6" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="S6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="T6" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="U6" s="24" t="s">
+      <c r="U6" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="V6" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="W6" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="X6" s="24" t="s">
+      <c r="X6" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="Y6" s="24" t="s">
+      <c r="Y6" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" s="24" t="s">
+      <c r="Z6" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AA6" s="24" t="s">
+      <c r="AA6" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AB6" s="24" t="s">
+      <c r="AB6" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="24" t="s">
+      <c r="AC6" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="AD6" s="24" t="s">
+      <c r="AD6" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="AE6" s="24" t="s">
+      <c r="AE6" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="AF6" s="24" t="s">
+      <c r="AF6" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="AG6" s="24" t="s">
+      <c r="AG6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="AH6" s="24" t="s">
+      <c r="AH6" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="AI6" s="24" t="s">
+      <c r="AI6" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="AJ6" s="24" t="s">
+      <c r="AJ6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="AK6" s="24" t="s">
+      <c r="AK6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="AL6" s="24" t="s">
+      <c r="AL6" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="AM6" s="24" t="s">
+      <c r="AM6" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AN6" s="25" t="s">
+      <c r="AN6" s="31" t="s">
         <v>84</v>
       </c>
       <c r="AME6" s="13"/>
@@ -1710,82 +1813,82 @@
       <c r="AMG6" s="13"/>
       <c r="AMH6" s="13"/>
       <c r="AMI6" s="13"/>
-      <c r="AMJ6" s="26"/>
+      <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="27" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+    <row r="7" s="13" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29" t="n">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="29" t="n">
+      <c r="L7" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="29" t="n">
+      <c r="M7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="29" t="n">
+      <c r="N7" s="33" t="n">
         <v>4</v>
       </c>
-      <c r="O7" s="29" t="n">
+      <c r="O7" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="R7" s="29" t="s">
+      <c r="R7" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="S7" s="29" t="s">
+      <c r="S7" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="T7" s="29" t="s">
+      <c r="T7" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="U7" s="29" t="s">
+      <c r="U7" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="V7" s="29" t="s">
+      <c r="V7" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="W7" s="29" t="s">
+      <c r="W7" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="X7" s="29" t="s">
+      <c r="X7" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="Y7" s="29" t="s">
+      <c r="Y7" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="Z7" s="29" t="s">
+      <c r="Z7" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="AA7" s="29" t="s">
+      <c r="AA7" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="AB7" s="29"/>
+      <c r="AB7" s="33"/>
       <c r="AC7" s="0"/>
       <c r="AD7" s="0"/>
       <c r="AE7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AE7"/>
+  <autoFilter ref="A6:AE6"/>
   <mergeCells count="15">
     <mergeCell ref="B3:J5"/>
     <mergeCell ref="K3:AA3"/>
@@ -1837,8 +1940,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1852,18 +1955,18 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1978,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1885,13 +1988,13 @@
       <c r="C2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="34" t="s">
         <v>101</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1905,36 +2008,36 @@
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="35" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H4"/>
+  <autoFilter ref="B3:H3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix #19822 - [Featutr] Update Citeo Export (FR)
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/fr/ExportCiteo.xlsx
@@ -5,22 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Eco emballage" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Matériaux" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$6</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="123">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -139,6 +131,18 @@
     <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AA"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
   </si>
   <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AB"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AC"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AD"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AE"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
     <t xml:space="preserve">bcpg:labelClaimList[bcpg:lclLabelClaim#bcpg:labelClaimCode=="ECO\\_PACK\\_50\\_RECYCLED"]_bcpg:lclClaimValue</t>
   </si>
   <si>
@@ -188,13 +192,19 @@
     <t xml:space="preserve">Quantités</t>
   </si>
   <si>
-    <t xml:space="preserve">Total de votre simulation 2021</t>
+    <t xml:space="preserve">Total de votre simulation 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Plastique</t>
   </si>
   <si>
+    <t xml:space="preserve">Métal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Papier-carton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verre</t>
   </si>
   <si>
     <t xml:space="preserve">Bouteille</t>
@@ -253,31 +263,40 @@
     <t xml:space="preserve">Briques</t>
   </si>
   <si>
-    <t xml:space="preserve">Verre</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bouteilles et flacons en PET clair</t>
   </si>
   <si>
-    <t xml:space="preserve">Bouteilles et flacons en PET foncé/opaque/coloré ou PE ou PP</t>
+    <t xml:space="preserve">Bouteilles et flacons en PET foncé/coloré</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouteille et flacon en PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouteille et flacon en PP</t>
   </si>
   <si>
     <t xml:space="preserve">Autres bouteilles hors PVC (PLA, complexe, ...)</t>
   </si>
   <si>
-    <t xml:space="preserve">Emballages rigides PE ou PP ou PET </t>
+    <t xml:space="preserve">Emballage rigide (hors B&amp;F) en PE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emballage rigide (hors B&amp;F) en PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emballage rigide (hors B&amp;F) en PET</t>
   </si>
   <si>
     <t xml:space="preserve">Emballages rigides en PS</t>
   </si>
   <si>
-    <t xml:space="preserve">Autres Emballages rigides hors PVC (PLA, complexe, ...)</t>
+    <t xml:space="preserve">Emballage complexe ou autres résines plastiques hors PVC</t>
   </si>
   <si>
     <t xml:space="preserve">Emballages souples en PE</t>
   </si>
   <si>
-    <t xml:space="preserve">Autres Emballages souples hors PVC (PET, PP, PLA, complexe, ...)</t>
+    <t xml:space="preserve">Emballage souple en PP</t>
   </si>
   <si>
     <t xml:space="preserve">Emballages contenant PVC (souples et rigides dont bouteilles)</t>
@@ -345,22 +364,37 @@
     <t xml:space="preserve">6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">6.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 .6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.3</t>
+    <t xml:space="preserve">6.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3.3</t>
   </si>
   <si>
     <t xml:space="preserve">6.5</t>
   </si>
   <si>
-    <t xml:space="preserve">6.6</t>
+    <t xml:space="preserve">6.6.2</t>
   </si>
   <si>
     <t xml:space="preserve">6.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6.1</t>
   </si>
   <si>
     <t xml:space="preserve">6.7</t>
@@ -419,7 +453,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -508,12 +542,6 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -616,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -693,19 +721,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
@@ -725,8 +740,12 @@
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -794,7 +813,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -847,39 +866,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -887,31 +902,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
@@ -919,15 +938,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="13" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="14" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -935,11 +954,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -952,6 +975,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF66CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1016,371 +1055,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 72222"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="0">
-          <a:gsLst>
-            <a:gs pos="80000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000"/>
-        </a:gradFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="23040" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Suivant</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 72222"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="0">
-          <a:gsLst>
-            <a:gs pos="80000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000"/>
-        </a:gradFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="23040" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Suivant</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 72222"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="0">
-          <a:gsLst>
-            <a:gs pos="80000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000"/>
-        </a:gradFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="23040" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Suivant</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 72222"/>
-            <a:gd name="adj2" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="0">
-          <a:gsLst>
-            <a:gs pos="80000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="ffffff"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000"/>
-        </a:gradFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="23040" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0" anchor="ctr">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr algn="ctr">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Suivant</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
@@ -1391,11 +1065,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
@@ -1406,18 +1080,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="17" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="17" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="30" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1427,7 +1102,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="27.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1512,16 +1187,28 @@
       <c r="AB2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="2"/>
+      <c r="AC2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="2"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1532,7 +1219,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -1550,43 +1237,45 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
-      <c r="AB3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="11" t="s">
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AG3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12" t="n">
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP3" s="12"/>
+      <c r="AQ3" s="12"/>
+      <c r="AR3" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="AME3" s="13"/>
-      <c r="AMF3" s="13"/>
-      <c r="AMG3" s="13"/>
-      <c r="AMH3" s="13"/>
-      <c r="AMI3" s="13"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="13" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="17" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1597,43 +1286,50 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="17"/>
-      <c r="X4" s="17"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="12"/>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="12"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1644,306 +1340,338 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
+      <c r="K5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="P5" s="18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
-      <c r="S5" s="18" t="s">
-        <v>42</v>
-      </c>
+      <c r="S5" s="18"/>
       <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y5" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
+      <c r="U5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="11"/>
+      <c r="AO5" s="11"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
     </row>
-    <row r="6" s="22" customFormat="true" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="23" t="s">
+    <row r="6" s="21" customFormat="true" ht="52.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="N6" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q6" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="S6" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="T6" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="U6" s="26" t="s">
+      <c r="P6" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="V6" s="26" t="s">
+      <c r="Q6" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="W6" s="26" t="s">
+      <c r="R6" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="X6" s="26" t="s">
+      <c r="S6" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="Y6" s="26" t="s">
+      <c r="T6" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" s="26" t="s">
+      <c r="U6" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AA6" s="26" t="s">
+      <c r="V6" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="AB6" s="27" t="s">
+      <c r="W6" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AC6" s="28" t="s">
+      <c r="X6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AD6" s="28" t="s">
+      <c r="Y6" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="AE6" s="28" t="s">
+      <c r="Z6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="AF6" s="28" t="s">
+      <c r="AA6" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="AG6" s="29" t="s">
+      <c r="AB6" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="AH6" s="29" t="s">
+      <c r="AC6" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="AI6" s="29" t="s">
+      <c r="AD6" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="AJ6" s="26" t="s">
+      <c r="AE6" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="AK6" s="30" t="s">
+      <c r="AF6" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="AL6" s="30" t="s">
+      <c r="AG6" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="AM6" s="30" t="s">
+      <c r="AH6" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="AN6" s="31" t="s">
+      <c r="AI6" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="AME6" s="13"/>
-      <c r="AMF6" s="13"/>
-      <c r="AMG6" s="13"/>
-      <c r="AMH6" s="13"/>
-      <c r="AMI6" s="13"/>
+      <c r="AJ6" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK6" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL6" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM6" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO6" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ6" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR6" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="AMG6" s="0"/>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="13" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33" t="n">
+    <row r="7" s="17" customFormat="true" ht="17.35" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="33" t="n">
+      <c r="L7" s="32" t="n">
         <v>2</v>
       </c>
-      <c r="M7" s="33" t="n">
+      <c r="M7" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="33" t="n">
+      <c r="N7" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="O7" s="33" t="n">
+      <c r="O7" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="P7" s="33" t="s">
-        <v>86</v>
+      <c r="P7" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="Q7" s="33" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="R7" s="33" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="S7" s="33" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="T7" s="33" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="U7" s="33" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="V7" s="33" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="W7" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="X7" s="33" t="s">
-        <v>93</v>
+        <v>102</v>
+      </c>
+      <c r="X7" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="Y7" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z7" s="33" t="s">
-        <v>95</v>
+        <v>104</v>
+      </c>
+      <c r="Z7" s="32" t="s">
+        <v>105</v>
       </c>
       <c r="AA7" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="0"/>
-      <c r="AD7" s="0"/>
-      <c r="AE7" s="0"/>
+        <v>106</v>
+      </c>
+      <c r="AB7" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC7" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD7" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE7" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF7" s="32"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AMG7" s="0"/>
+      <c r="AMH7" s="0"/>
+      <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AE6"/>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="B3:J5"/>
-    <mergeCell ref="K3:AA3"/>
-    <mergeCell ref="AB3:AB5"/>
-    <mergeCell ref="AC3:AD5"/>
-    <mergeCell ref="AE3:AF5"/>
-    <mergeCell ref="AG3:AI5"/>
-    <mergeCell ref="AJ3:AJ5"/>
-    <mergeCell ref="AK3:AN5"/>
-    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="K3:AE3"/>
+    <mergeCell ref="AF3:AF5"/>
+    <mergeCell ref="AG3:AH5"/>
+    <mergeCell ref="AI3:AJ5"/>
+    <mergeCell ref="AK3:AM5"/>
+    <mergeCell ref="AN3:AN5"/>
+    <mergeCell ref="AO3:AR5"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Y5:AA5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="U5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AC5:AE5"/>
     <mergeCell ref="B7:J7"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez OUI si votre emballage est en papier-carton recyclé et qu'il contient plus de 50% de recyclé. &#10;Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Indiquez OUI si votre emballage est en papier-carton recyclé et qu'il contient plus de 50% de recyclé.  Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AF6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- Triman uniquement 5%&#10;- Triman + off-pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place : - Consigne 8% (On-pack/notice) - Off-Pack 4% - Consigne + Off-Pack 12% - Triman uniquement 5% - Triman + off-pack 9% Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AG6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action mise en place :&#10;- Réduction de poids 8%&#10;- Suppression d’une unité 8%&#10;Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Indiquez le type d'action mise en place : - Réduction de poids 8% - Suppression d’une unité 8% Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- QR code 4%&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- QR Code + Off-Pack 8%&#10;- Triman uniquement 5%&#10;- Triman + Off-Pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE6 AG6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place : - Consigne 8% (On-pack/notice) - QR code 4% - Off-Pack 4% - Consigne + Off-Pack 12% - QR Code + Off-Pack 8% - Triman uniquement 5% - Triman + Off-Pack 9% Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AI6 AK6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Choisissez dans la liste déroulante.&#10;Sinon laissez la case vide.&#10;" promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH6:AI6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Choisissez dans la liste déroulante. Sinon laissez la case vide. " promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AL6:AM6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le nombre d'Unités de Vente Consommateur (UVC) mises sur le marché français." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Indiquez le nombre d'Unités de Vente Consommateur (UVC) mises sur le marché français." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AN6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AN3" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AR3" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1954,31 +1682,32 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1986,55 +1715,55 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>101</v>
+        <v>114</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>115</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>108</v>
+        <v>34</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B3:H3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>